<commit_message>
Melhorias no código (P/Sonar)
</commit_message>
<xml_diff>
--- a/LOG/Inspeção App-RSI.xlsx
+++ b/LOG/Inspeção App-RSI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helio.franca\Documents\GitHub\RSI\LOG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{27571CEA-DE6A-417C-A0E6-F8093D7200BF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{755B654E-F37D-4CB8-9E1B-4EDAA14ECE7B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="50">
   <si>
     <t>Gestor</t>
   </si>
@@ -243,12 +243,103 @@
       <t>A</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>451</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>A</t>
+    </r>
+  </si>
+  <si>
+    <t>30.8%</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <r>
+      <t>450</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>A</t>
+    </r>
+  </si>
+  <si>
+    <t>30.3%</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <r>
+      <t>439</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>A</t>
+    </r>
+  </si>
+  <si>
+    <t>30.1%</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <r>
+      <t>435</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>A</t>
+    </r>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +377,24 @@
     <font>
       <sz val="6"/>
       <color theme="3"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF444444"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF444444"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -334,7 +443,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -371,43 +480,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -429,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -449,30 +521,9 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -481,6 +532,30 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -796,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5918C00F-7599-4FB4-AA5D-6C2FEA5A9C96}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -810,18 +885,18 @@
     <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="3">
         <f>SUBTOTAL(2,D4:D99)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3">
         <f>SUBTOTAL(9,E4:E99)</f>
-        <v>29283</v>
+        <v>52667</v>
       </c>
       <c r="F1" s="3">
         <f>SUBTOTAL(9,F4:F99)</f>
@@ -829,22 +904,22 @@
       </c>
       <c r="G1" s="3">
         <f>SUBTOTAL(9,G4:G99)</f>
-        <v>334</v>
+        <v>560</v>
       </c>
       <c r="H1" s="3">
         <f>SUBTOTAL(9,H4:H99)</f>
-        <v>1191</v>
+        <v>1959</v>
       </c>
       <c r="I1" s="3">
         <f>SUBTOTAL(9,I4:I99)</f>
-        <v>1034</v>
+        <v>1787</v>
       </c>
       <c r="J1" s="4">
         <f>100%-SUM((F1/E1)*10,(G1/E1)*5,(H1/E1),(I1/E1)*0.1)</f>
-        <v>0.88988833111361543</v>
+        <v>0.90131011829039054</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -854,15 +929,19 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="6"/>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -893,350 +972,606 @@
       <c r="J3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="7">
         <v>0</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="7" t="s">
         <v>28</v>
       </c>
+      <c r="Q3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="7">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="14">
         <v>0</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="15">
         <v>43347</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="14">
         <v>5865</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="14">
         <v>18</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="14">
         <v>67</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="14">
         <v>240</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="14">
         <v>207</v>
       </c>
-      <c r="J4" s="9">
-        <f>100%-SUM((F4/E4)*10,(G4/E4)*5,(H4/E4),(I4/E4)*0.1)</f>
+      <c r="J4" s="16">
+        <f t="shared" ref="J4:J9" si="0">100%-SUM((F4/E4)*10,(G4/E4)*5,(H4/E4),(I4/E4)*0.1)</f>
         <v>0.86774083546462055</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="15" t="s">
+      <c r="N4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="15" t="s">
+      <c r="P4" s="8" t="s">
         <v>31</v>
       </c>
+      <c r="Q4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="15">
         <v>43347</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="14">
         <v>5865</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="14">
         <v>7</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="14">
         <v>67</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="14">
         <v>240</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="14">
         <v>207</v>
       </c>
-      <c r="J5" s="9">
-        <f>100%-SUM((F5/E5)*10,(G5/E5)*5,(H5/E5),(I5/E5)*0.1)</f>
+      <c r="J5" s="16">
+        <f t="shared" si="0"/>
         <v>0.88649616368286444</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="M5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="O5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="16" t="s">
+      <c r="P5" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="Q5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" s="12" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="15">
         <v>43347</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="14">
         <v>5859</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="14">
         <v>1</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="14">
         <v>67</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="14">
         <v>240</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="14">
         <v>207</v>
       </c>
-      <c r="J6" s="9">
-        <f>100%-SUM((F6/E6)*10,(G6/E6)*5,(H6/E6),(I6/E6)*0.1)</f>
+      <c r="J6" s="16">
+        <f t="shared" si="0"/>
         <v>0.89662058371735787</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="15" t="s">
+      <c r="N6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="P6" s="15" t="s">
+      <c r="P6" s="8" t="s">
         <v>34</v>
       </c>
+      <c r="Q6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="15">
         <v>43347</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="14">
         <v>5848</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="14">
         <v>0</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="14">
         <v>67</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="14">
         <v>240</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="14">
         <v>207</v>
       </c>
-      <c r="J7" s="9">
-        <f>100%-SUM((F7/E7)*10,(G7/E7)*5,(H7/E7),(I7/E7)*0.1)</f>
+      <c r="J7" s="16">
+        <f t="shared" si="0"/>
         <v>0.8981361149110807</v>
       </c>
-      <c r="L7" s="16" t="s">
+      <c r="L7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="M7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="P7" s="9" t="s">
         <v>17</v>
       </c>
+      <c r="Q7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="10">
-        <v>43347</v>
-      </c>
-      <c r="E8" s="8">
+      <c r="D8" s="15">
+        <v>43348</v>
+      </c>
+      <c r="E8" s="14">
         <v>5846</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="14">
         <v>0</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="14">
         <v>66</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="14">
         <v>231</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="14">
         <v>206</v>
       </c>
-      <c r="J8" s="9">
-        <f>100%-SUM((F8/E8)*10,(G8/E8)*5,(H8/E8),(I8/E8)*0.1)</f>
+      <c r="J8" s="16">
+        <f t="shared" si="0"/>
         <v>0.90051317139924736</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="M8" s="15" t="s">
+      <c r="M8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="N8" s="15" t="s">
+      <c r="N8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O8" s="15" t="s">
+      <c r="O8" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P8" s="15" t="s">
+      <c r="P8" s="8" t="s">
         <v>37</v>
       </c>
+      <c r="Q8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="R8" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="T8" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="L9" s="16" t="s">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="15">
+        <v>43349</v>
+      </c>
+      <c r="E9" s="14">
+        <v>5846</v>
+      </c>
+      <c r="F9" s="14">
+        <v>0</v>
+      </c>
+      <c r="G9" s="14">
+        <v>64</v>
+      </c>
+      <c r="H9" s="14">
+        <v>193</v>
+      </c>
+      <c r="I9" s="14">
+        <v>187</v>
+      </c>
+      <c r="J9" s="16">
+        <f t="shared" si="0"/>
+        <v>0.90904892234006163</v>
+      </c>
+      <c r="L9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="16" t="s">
+      <c r="N9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="O9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="P9" s="9" t="s">
         <v>18</v>
       </c>
+      <c r="Q9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="R9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="S9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="T9" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="L10" s="15" t="s">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="15">
+        <v>43349</v>
+      </c>
+      <c r="E10" s="14">
+        <v>5846</v>
+      </c>
+      <c r="F10" s="14">
+        <v>0</v>
+      </c>
+      <c r="G10" s="14">
+        <v>62</v>
+      </c>
+      <c r="H10" s="14">
+        <v>193</v>
+      </c>
+      <c r="I10" s="14">
+        <v>188</v>
+      </c>
+      <c r="J10" s="16">
+        <f t="shared" ref="J10" si="1">100%-SUM((F10/E10)*10,(G10/E10)*5,(H10/E10),(I10/E10)*0.1)</f>
+        <v>0.91074238795757778</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N10" s="15" t="s">
+      <c r="N10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="15" t="s">
+      <c r="O10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="P10" s="15" t="s">
+      <c r="P10" s="8" t="s">
         <v>13</v>
       </c>
+      <c r="Q10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="T10" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="L11" s="17" t="s">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="15">
+        <v>43349</v>
+      </c>
+      <c r="E11" s="14">
+        <v>5846</v>
+      </c>
+      <c r="F11" s="14">
+        <v>0</v>
+      </c>
+      <c r="G11" s="14">
+        <v>51</v>
+      </c>
+      <c r="H11" s="14">
+        <v>193</v>
+      </c>
+      <c r="I11" s="14">
+        <v>188</v>
+      </c>
+      <c r="J11" s="16">
+        <f t="shared" ref="J11" si="2">100%-SUM((F11/E11)*10,(G11/E11)*5,(H11/E11),(I11/E11)*0.1)</f>
+        <v>0.92015053027711258</v>
+      </c>
+      <c r="L11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="M11" s="17" t="s">
+      <c r="M11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="N11" s="17" t="s">
+      <c r="N11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="O11" s="17" t="s">
+      <c r="O11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="P11" s="17" t="s">
+      <c r="P11" s="10" t="s">
         <v>19</v>
       </c>
+      <c r="Q11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="R11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="S11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="T11" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="L12" s="15" t="s">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="15">
+        <v>43349</v>
+      </c>
+      <c r="E12" s="14">
+        <v>5846</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0</v>
+      </c>
+      <c r="G12" s="14">
+        <v>49</v>
+      </c>
+      <c r="H12" s="14">
+        <v>189</v>
+      </c>
+      <c r="I12" s="14">
+        <v>190</v>
+      </c>
+      <c r="J12" s="16">
+        <f t="shared" ref="J12" si="3">100%-SUM((F12/E12)*10,(G12/E12)*5,(H12/E12),(I12/E12)*0.1)</f>
+        <v>0.92251111871365032</v>
+      </c>
+      <c r="L12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N12" s="15" t="s">
+      <c r="N12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="O12" s="15" t="s">
+      <c r="O12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="P12" s="15" t="s">
+      <c r="P12" s="8" t="s">
         <v>15</v>
       </c>
+      <c r="Q12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S12" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T12" s="11" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="L13" s="17" t="s">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="L13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="M13" s="17" t="s">
+      <c r="M13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="N13" s="17" t="s">
+      <c r="N13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O13" s="17" t="s">
+      <c r="O13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P13" s="17" t="s">
+      <c r="P13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="R13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="S13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="T13" s="13" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="L2:T2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>